<commit_message>
project 2 mostly completed
</commit_message>
<xml_diff>
--- a/projects/project-2-master/submissions/submit_log.xlsx
+++ b/projects/project-2-master/submissions/submit_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/genebob/Dropbox/ga/dsir-1213/submissions/projects/project-2-master/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90ED0BF2-673D-F44D-8924-9851C65F2BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECFB542-9F1C-0E4E-AF47-221355571FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9920" yWindow="6560" windowWidth="28040" windowHeight="15880" xr2:uid="{68CD0C34-31B7-8D49-8447-1DEFF045D898}"/>
+    <workbookView xWindow="5640" yWindow="4280" windowWidth="28040" windowHeight="15880" xr2:uid="{68CD0C34-31B7-8D49-8447-1DEFF045D898}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>file_name</t>
   </si>
@@ -79,6 +79,21 @@
   </si>
   <si>
     <t>ridge6_submit.csv</t>
+  </si>
+  <si>
+    <t>['n_grnhill', 'n_greens', 'n_blueste', 'n_npkvill', 'n_veenker', 'n_brdale', 'n_blmngtn', 'n_meadowv', 'n_clearcr', 'n_swisu', 'n_stonebr', 'n_timber', 'n_noridge', 'n_idotrr', 'n_crawfor', 'n_brkside', 'n_mitchel', 'n_sawyerw', 'n_nwames', 'n_sawyer', 'n_gilbert', 'n_nridght', 'n_somerst', 'n_edwards', 'n_oldtown', 'n_collgcr', 'n_names', 'type_twn', 'type_sf', 'type_twn_end', 'gar_attached', 'gar_detached', 'gar_builtin', 'gar_basement', 'gar_2types', 'gar_carport', 'quality', 'gr_living_sqft', 'kitchen_qual', 'garage_sqft', 'garage_size', 'total_basement_sqft', 'sqft_1', 'basement_qual', 'year', 'garage_finish', 'garage_year', 'remod_year', 'baths', 'fireplace_qual', 'full_bath', 'mas_vnr_area', 'foundation', 'fireplaces', 'heating_qc', 'basement_exposure', 'basement_fin_sqft_1', 'gar_attached', 'sale_type', 'basement_fin_1', 'shape', 'fence', 'kitchen', 'conds', 'condition']</t>
+  </si>
+  <si>
+    <t>ridge7_submit.csv</t>
+  </si>
+  <si>
+    <t>ridge8_submit.csv</t>
+  </si>
+  <si>
+    <t>ridge9_submit.csv</t>
+  </si>
+  <si>
+    <t>['n_grnhill', 'n_greens', 'n_blueste', 'n_npkvill', 'n_veenker', 'n_brdale', 'n_blmngtn', 'n_meadowv', 'n_clearcr', 'n_swisu', 'n_stonebr', 'n_timber', 'n_noridge', 'n_idotrr', 'n_crawfor', 'n_brkside', 'n_mitchel', 'n_sawyerw', 'n_nwames', 'n_sawyer', 'n_gilbert', 'n_nridght', 'n_somerst', 'n_edwards', 'n_oldtown', 'n_collgcr', 'n_names', 'type_twn', 'type_sf', 'type_twn_end', 'gar_attached', 'gar_detached', 'gar_builtin', 'gar_basement', 'gar_2types', 'gar_carport', 'quality', 'gr_living_sqft', 'kitchen_qual', 'garage_sqft', 'garage_size', 'total_basement_sqft', 'sqft_1', 'basement_qual', 'year', 'garage_finish', 'garage_year', 'remod_year', 'baths', 'fireplace_qual', 'full_bath', 'mas_vnr_area', 'foundation', 'fireplaces', 'heating_qc', 'basement_exposure', 'basement_fin_sqft_1', 'gar_attached', 'sale_type', 'basement_fin_1', 'shape', 'fence', 'kitchen', 'conds', 'condition', 'contour_hill', 'contour_bank', 'contour_level', 'alley_gravel', 'alley_pave', 'street_material', 'lot_sqft', 'electrical', 'heating', 'basement_fin_2', 'sold_year_mo', 'basement_fin_sqft_2']</t>
   </si>
 </sst>
 </file>
@@ -430,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{510F2AA6-F9C5-FA4E-98AC-91077A685CAB}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,6 +572,57 @@
         <v>10</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>500</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>250</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>500</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Project 2 presentation updated
</commit_message>
<xml_diff>
--- a/projects/project-2-master/submissions/submit_log.xlsx
+++ b/projects/project-2-master/submissions/submit_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/genebob/Dropbox/ga/dsir-1213/submissions/projects/project-2-master/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECFB542-9F1C-0E4E-AF47-221355571FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51FAC9B-6D97-D14B-8FAC-17DB67F360D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5640" yWindow="4280" windowWidth="28040" windowHeight="15880" xr2:uid="{68CD0C34-31B7-8D49-8447-1DEFF045D898}"/>
+    <workbookView xWindow="5460" yWindow="5240" windowWidth="28040" windowHeight="15880" xr2:uid="{68CD0C34-31B7-8D49-8447-1DEFF045D898}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="28">
   <si>
     <t>file_name</t>
   </si>
@@ -94,6 +94,48 @@
   </si>
   <si>
     <t>['n_grnhill', 'n_greens', 'n_blueste', 'n_npkvill', 'n_veenker', 'n_brdale', 'n_blmngtn', 'n_meadowv', 'n_clearcr', 'n_swisu', 'n_stonebr', 'n_timber', 'n_noridge', 'n_idotrr', 'n_crawfor', 'n_brkside', 'n_mitchel', 'n_sawyerw', 'n_nwames', 'n_sawyer', 'n_gilbert', 'n_nridght', 'n_somerst', 'n_edwards', 'n_oldtown', 'n_collgcr', 'n_names', 'type_twn', 'type_sf', 'type_twn_end', 'gar_attached', 'gar_detached', 'gar_builtin', 'gar_basement', 'gar_2types', 'gar_carport', 'quality', 'gr_living_sqft', 'kitchen_qual', 'garage_sqft', 'garage_size', 'total_basement_sqft', 'sqft_1', 'basement_qual', 'year', 'garage_finish', 'garage_year', 'remod_year', 'baths', 'fireplace_qual', 'full_bath', 'mas_vnr_area', 'foundation', 'fireplaces', 'heating_qc', 'basement_exposure', 'basement_fin_sqft_1', 'gar_attached', 'sale_type', 'basement_fin_1', 'shape', 'fence', 'kitchen', 'conds', 'condition', 'contour_hill', 'contour_bank', 'contour_level', 'alley_gravel', 'alley_pave', 'street_material', 'lot_sqft', 'electrical', 'heating', 'basement_fin_2', 'sold_year_mo', 'basement_fin_sqft_2']</t>
+  </si>
+  <si>
+    <t>ridge10_submit.csv</t>
+  </si>
+  <si>
+    <t>ridge11_submit.csv</t>
+  </si>
+  <si>
+    <t>['n_grnhill', 'n_greens', 'n_blueste', 'n_npkvill', 'n_veenker', 'n_brdale', 'n_blmngtn', 'n_meadowv', 'n_clearcr', 'n_swisu', 'n_stonebr', 'n_timber', 
+'n_noridge', 'n_idotrr', 'n_crawfor', 'n_brkside', 'n_mitchel', 'n_sawyerw', 'n_nwames', 'n_sawyer', 'n_gilbert', 'n_nridght', 'n_somerst', 'n_edwards', 'n_oldtown', 
+'n_collgcr', 'n_names', 'type_twn', 'type_sf', 'type_twn_end', 'gar_attached', 'gar_detached', 'gar_builtin', 'gar_basement', 'gar_2types', 'gar_carport', 'quality', 
+'gr_living_sqft', 'kitchen_qual', 'garage_sqft', 'garage_size', 'total_basement_sqft', 'sqft_1', 'basement_qual', 'year', 'garage_finish', 'garage_year', 'remod_year', 
+'baths', 'fireplace_qual', 'full_bath', 'mas_vnr_area', 'foundation', 'fireplaces', 'heating_qc', 'basement_exposure', 'basement_fin_sqft_1', 'gar_attached', 'sale_type', 
+'basement_fin_1', 'shape', 'fence', 'kitchen', 'conds', 'condition', 'contour_hill', 'contour_bank', 'contour_level', 'alley_gravel', 'alley_pave', 'street_material', 
+'low_qual_sqft', 'lot_sqft', 'electrical', 'heating', 'basement_fin_2', 'sold_year_mo', 'basement_fin_sqft_2']</t>
+  </si>
+  <si>
+    <t>ridge12_submit.csv</t>
+  </si>
+  <si>
+    <t>['n_grnhill', 'n_greens', 'n_blueste', 'n_npkvill', 'n_veenker', 'n_brdale', 'n_blmngtn', 'n_meadowv', 'n_clearcr', 'n_swisu', 'n_stonebr', 'n_timber', 
+'n_noridge', 'n_idotrr', 'n_crawfor', 'n_brkside', 'n_mitchel', 'n_sawyerw', 'n_nwames', 'n_sawyer', 'n_gilbert', 'n_nridght', 'n_somerst', 'n_edwards', 'n_oldtown', 
+'n_collgcr', 'n_names', 'type_twn', 'type_sf', 'type_twn_end', 'gar_attached', 'gar_detached', 'gar_builtin', 'gar_basement', 'gar_2types', 'gar_carport', 'quality', 
+'gr_living_sqft', 'kitchen_qual', 'garage_sqft', 'garage_size', 'total_basement_sqft', 'sqft_1', 'basement_qual', 'year', 'garage_finish', 'garage_year', 'remod_year', 
+'baths', 'fireplace_qual', 'full_bath', 'mas_vnr_area', 'foundation', 'fireplaces', 'heating_qc', 'basement_exposure', 'basement_fin_sqft_1', 'gar_attached', 'sale_type', 
+'basement_fin_1', 'shape', 'fence', 'kitchen', 'conds', 'condition', 'contour_hill', 'contour_bank', 'contour_level', 'alley_gravel', 'alley_pave', 'street_material', 
+'low_qual_sqft', 'lot_sqft', 'electrical', 'heating', 'basement_fin_2']</t>
+  </si>
+  <si>
+    <t>ridge13_submit.csv</t>
+  </si>
+  <si>
+    <t>ridge14_submit.csv</t>
+  </si>
+  <si>
+    <t>['n_grnhill', 'n_greens', 'n_blueste', 'n_npkvill', 'n_veenker', 'n_brdale', 'n_blmngtn', 'n_meadowv', 'n_clearcr', 'n_swisu', 'n_stonebr', 'n_timber', 
+'n_noridge', 'n_idotrr', 'n_crawfor', 'n_brkside', 'n_mitchel', 'n_sawyerw', 'n_nwames', 'n_sawyer', 'n_gilbert', 'n_nridght', 'n_somerst', 'n_edwards', 'n_oldtown', 'n_collgcr', 
+'n_names', 'type_twn', 'type_sf', 'type_twn_end', 'gar_attached', 'gar_detached', 'gar_builtin', 'gar_basement', 'gar_2types', 'gar_carport', 'quality', 'gr_living_sqft', 
+'kitchen_qual', 'garage_sqft', 'garage_size', 'total_basement_sqft', 'sqft_1', 'basement_qual', 'year', 'garage_finish', 'garage_year', 'remod_year', 'baths', 'fireplace_qual', 
+'full_bath', 'mas_vnr_area', 'foundation', 'fireplaces', 'heating_qc', 'basement_exposure', 'basement_fin_sqft_1', 'gar_attached', 'sale_type', 'basement_fin_1', 'shape', 'fence', 
+'kitchen', 'conds', 'condition', 'contour_hill', 'contour_bank', 'contour_level', 'alley_gravel', 'alley_pave', 'street_material', 'lot_sqft', 'electrical', 'heating', 
+'basement_fin_2', 'sold_year_mo', 'basement_fin_sqft_2']</t>
   </si>
 </sst>
 </file>
@@ -129,8 +171,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{510F2AA6-F9C5-FA4E-98AC-91077A685CAB}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,6 +668,91 @@
         <v>9</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>1000</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>900</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>850</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>800</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>850</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>